<commit_message>
ccbottlersus fix template and comment
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS_SAND/Data/KPITemplateV3.xlsx
+++ b/Projects/CCBOTTLERSUS_SAND/Data/KPITemplateV3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,24 +27,28 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$O$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$O$70</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$O$70</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$O$70</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Availability!$A$1:$J$64</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">SOS!$A$1:$I$10</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">SOS!$A$1:$I$10</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">SOS!$A$1:$I$10</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">SOS!$A$1:$I$10</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">SOS!$A$1:$I$10</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">SOS!$A$1:$I$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">SOS!$A$1:$I$10</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Survey!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1207,19 +1211,19 @@
   </sheetPr>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G39" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.8461538461539"/>
     <col collapsed="false" hidden="false" max="11" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -3402,13 +3406,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H64" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="H64" activeCellId="0" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="7" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="1017" min="4" style="7" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.78542510121457"/>
   </cols>
@@ -20864,20 +20868,20 @@
   <dimension ref="1:22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -21494,7 +21498,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -21503,8 +21507,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -21694,15 +21698,17 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B27" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4858299595142"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22103,7 +22109,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22113,7 +22119,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7125506072874"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="46.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -22164,13 +22170,13 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>

</xml_diff>